<commit_message>
Presentation updated with schedule and objecties
</commit_message>
<xml_diff>
--- a/presentation/Reference_Tables_11-Jul-2023.xlsx
+++ b/presentation/Reference_Tables_11-Jul-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB098A05-FF08-44E4-B964-F4ED200BFBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC856A7-DE0C-4904-B563-4AA86223A346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="436" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="423" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LATEX" sheetId="27" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Super-models_large_table" sheetId="34" r:id="rId5"/>
     <sheet name="Super models" sheetId="33" r:id="rId6"/>
     <sheet name="t-test" sheetId="35" r:id="rId7"/>
+    <sheet name="Algorithm timelines" sheetId="36" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="144">
   <si>
     <t>environment_info</t>
   </si>
@@ -462,6 +463,41 @@
   </si>
   <si>
     <t>F Beta (0.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monte Carlo Sampling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Temporal Difference Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Q-Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REINFORCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DQN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A3C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PPO </t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Monte Carlo Sampling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Temporal
+ Difference
+ Learning</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1168,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1188,15 +1224,18 @@
     <xf numFmtId="164" fontId="26" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1261,6 +1300,524 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>308741</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>72259</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>308741</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>118241</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB463A9B-3072-3F80-1B7A-F2A46A845791}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6490138" y="72259"/>
+          <a:ext cx="0" cy="3284482"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261342</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70168</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>359876</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>168702</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBD05F38-0E83-5C1D-DBB5-0E172ACE0AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6430299" y="260668"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261932</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>53716</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>360466</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C93B145-CB00-435D-901D-C0099D61DC6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6430889" y="625216"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>262798</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50253</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361332</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>148787</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D85FB4BE-8F3F-479B-AFE3-FCD0B394191E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6431755" y="1764753"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>262798</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>61683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361332</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>160217</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B767432B-A736-4E03-999F-8321CC204BFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6434998" y="1966683"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>258988</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>357522</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>137357</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Oval 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E893CA28-A295-4FEA-87EB-F09D42F49609}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6431188" y="2705823"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261313</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>50982</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>359847</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>149516</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Oval 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CCDCD2E-DD55-4F46-AFFE-A588EB6B0746}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6439983" y="2908482"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>262387</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>46726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>360921</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>145260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Oval 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5557E639-F8B8-48CC-ACAE-75E7D0A6A057}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6441057" y="3094726"/>
+          <a:ext cx="98534" cy="98534"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5066,7 +5623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905A37E9-AAF7-4185-BB7B-87043DE103AD}">
   <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -5105,53 +5662,53 @@
       <c r="M2" s="17"/>
     </row>
     <row r="3" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="37" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="37" t="s">
+      <c r="G3" s="41"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="37" t="s">
+      <c r="J3" s="41"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="M3" s="37"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="36"/>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="39" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="39" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="39" t="s">
+      <c r="K4" s="39"/>
+      <c r="L4" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="38" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5225,31 +5782,31 @@
       <c r="B7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>0.47210000000000002</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="39">
         <v>0.1444</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40">
+      <c r="E7" s="39"/>
+      <c r="F7" s="39">
         <v>0.31559999999999999</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="39">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40">
+      <c r="H7" s="39"/>
+      <c r="I7" s="39">
         <v>0.34489999999999998</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="39">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40">
+      <c r="K7" s="39"/>
+      <c r="L7" s="39">
         <v>0.39290000000000003</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="39">
         <v>0.1046</v>
       </c>
       <c r="O7" t="str">
@@ -5261,31 +5818,31 @@
       <c r="B8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>0.68679999999999997</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="40">
         <v>5.9400000000000001E-2</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41">
+      <c r="E8" s="40"/>
+      <c r="F8" s="40">
         <v>0.62919999999999998</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="40">
         <v>5.0900000000000001E-2</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41">
+      <c r="H8" s="40"/>
+      <c r="I8" s="40">
         <v>0.60919999999999996</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="40">
         <v>4.9700000000000001E-2</v>
       </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41">
+      <c r="K8" s="40"/>
+      <c r="L8" s="40">
         <v>0.63060000000000005</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="40">
         <v>5.1799999999999999E-2</v>
       </c>
       <c r="O8" s="16" t="str">
@@ -5394,53 +5951,53 @@
       <c r="M13" s="17"/>
     </row>
     <row r="14" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="37" t="s">
+      <c r="D14" s="41"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="37" t="s">
+      <c r="G14" s="41"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="37" t="s">
+      <c r="J14" s="41"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="M14" s="37"/>
+      <c r="M14" s="41"/>
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="36"/>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="39" t="s">
+      <c r="E15" s="39"/>
+      <c r="F15" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="39" t="s">
+      <c r="H15" s="39"/>
+      <c r="I15" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="39" t="s">
+      <c r="K15" s="39"/>
+      <c r="L15" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="M15" s="39" t="s">
+      <c r="M15" s="38" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5514,31 +6071,31 @@
       <c r="B18" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="39">
         <v>0.49980000000000002</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="39">
         <v>0.1779</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40">
+      <c r="E18" s="39"/>
+      <c r="F18" s="39">
         <v>0.2145</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="39">
         <v>8.14E-2</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40">
+      <c r="H18" s="39"/>
+      <c r="I18" s="39">
         <v>0.28449999999999998</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="39">
         <v>9.9299999999999999E-2</v>
       </c>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40">
+      <c r="K18" s="39"/>
+      <c r="L18" s="39">
         <v>0.37040000000000001</v>
       </c>
-      <c r="M18" s="40">
+      <c r="M18" s="39">
         <v>0.1221</v>
       </c>
       <c r="O18" t="str">
@@ -5550,31 +6107,31 @@
       <c r="B19" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="40">
         <v>0.80589999999999995</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="40">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40">
         <v>0.9153</v>
       </c>
-      <c r="G19" s="41">
+      <c r="G19" s="40">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41">
+      <c r="H19" s="40"/>
+      <c r="I19" s="40">
         <v>0.84140000000000004</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="40">
         <v>3.5400000000000001E-2</v>
       </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41">
+      <c r="K19" s="40"/>
+      <c r="L19" s="40">
         <v>0.81559999999999999</v>
       </c>
-      <c r="M19" s="41">
+      <c r="M19" s="40">
         <v>3.6900000000000002E-2</v>
       </c>
       <c r="O19" s="16" t="str">
@@ -5673,53 +6230,53 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="37" t="s">
+      <c r="D26" s="41"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="37" t="s">
+      <c r="G26" s="41"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="37" t="s">
+      <c r="J26" s="41"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="M26" s="37"/>
+      <c r="M26" s="41"/>
     </row>
     <row r="27" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="36"/>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="39" t="s">
+      <c r="E27" s="39"/>
+      <c r="F27" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H27" s="40"/>
-      <c r="I27" s="39" t="s">
+      <c r="H27" s="39"/>
+      <c r="I27" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="K27" s="40"/>
-      <c r="L27" s="39" t="s">
+      <c r="K27" s="39"/>
+      <c r="L27" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="M27" s="39" t="s">
+      <c r="M27" s="38" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5793,31 +6350,31 @@
       <c r="B30" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="40">
+      <c r="C30" s="39">
         <v>0.44969999999999999</v>
       </c>
-      <c r="D30" s="40">
+      <c r="D30" s="39">
         <v>0.1459</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40">
+      <c r="E30" s="39"/>
+      <c r="F30" s="39">
         <v>0.31390000000000001</v>
       </c>
-      <c r="G30" s="40">
+      <c r="G30" s="39">
         <v>8.1500000000000003E-2</v>
       </c>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40">
+      <c r="H30" s="39"/>
+      <c r="I30" s="39">
         <v>0.33300000000000002</v>
       </c>
-      <c r="J30" s="40">
+      <c r="J30" s="39">
         <v>8.6599999999999996E-2</v>
       </c>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40">
+      <c r="K30" s="39"/>
+      <c r="L30" s="39">
         <v>0.37409999999999999</v>
       </c>
-      <c r="M30" s="40">
+      <c r="M30" s="39">
         <v>0.1017</v>
       </c>
       <c r="O30" t="str">
@@ -5829,31 +6386,31 @@
       <c r="B31" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="40">
         <v>0.60499999999999998</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="40">
         <v>4.6199999999999998E-2</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41">
+      <c r="E31" s="40"/>
+      <c r="F31" s="40">
         <v>0.60329999999999995</v>
       </c>
-      <c r="G31" s="41">
+      <c r="G31" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41">
+      <c r="H31" s="40"/>
+      <c r="I31" s="40">
         <v>0.56979999999999997</v>
       </c>
-      <c r="J31" s="41">
+      <c r="J31" s="40">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41">
+      <c r="K31" s="40"/>
+      <c r="L31" s="40">
         <v>0.57620000000000005</v>
       </c>
-      <c r="M31" s="41">
+      <c r="M31" s="40">
         <v>4.0300000000000002E-2</v>
       </c>
       <c r="O31" s="16" t="str">
@@ -5878,53 +6435,53 @@
       <c r="M34" s="17"/>
     </row>
     <row r="35" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="37" t="s">
+      <c r="D35" s="41"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="37" t="s">
+      <c r="G35" s="41"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="J35" s="37"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="37" t="s">
+      <c r="J35" s="41"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="M35" s="37"/>
+      <c r="M35" s="41"/>
     </row>
     <row r="36" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="39" t="s">
+      <c r="D36" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="39" t="s">
+      <c r="E36" s="39"/>
+      <c r="F36" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="G36" s="39" t="s">
+      <c r="G36" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="39" t="s">
+      <c r="H36" s="39"/>
+      <c r="I36" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="J36" s="39" t="s">
+      <c r="J36" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="K36" s="40"/>
-      <c r="L36" s="39" t="s">
+      <c r="K36" s="39"/>
+      <c r="L36" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="M36" s="39" t="s">
+      <c r="M36" s="38" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5998,31 +6555,31 @@
       <c r="B39" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="40">
+      <c r="C39" s="39">
         <v>0.51149999999999995</v>
       </c>
-      <c r="D39" s="40">
+      <c r="D39" s="39">
         <v>0.1067</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40">
+      <c r="E39" s="39"/>
+      <c r="F39" s="39">
         <v>0.42149999999999999</v>
       </c>
-      <c r="G39" s="40">
+      <c r="G39" s="39">
         <v>0.1074</v>
       </c>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40">
+      <c r="H39" s="39"/>
+      <c r="I39" s="39">
         <v>0.44080000000000003</v>
       </c>
-      <c r="J39" s="40">
+      <c r="J39" s="39">
         <v>9.5799999999999996E-2</v>
       </c>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40">
+      <c r="K39" s="39"/>
+      <c r="L39" s="39">
         <v>0.47149999999999997</v>
       </c>
-      <c r="M39" s="40">
+      <c r="M39" s="39">
         <v>9.5600000000000004E-2</v>
       </c>
       <c r="O39" t="str">
@@ -6034,31 +6591,31 @@
       <c r="B40" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="41">
+      <c r="C40" s="40">
         <v>0.81279999999999997</v>
       </c>
-      <c r="D40" s="41">
+      <c r="D40" s="40">
         <v>0.1187</v>
       </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41">
+      <c r="E40" s="40"/>
+      <c r="F40" s="40">
         <v>0.42070000000000002</v>
       </c>
-      <c r="G40" s="41">
+      <c r="G40" s="40">
         <v>7.8899999999999998E-2</v>
       </c>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41">
+      <c r="H40" s="40"/>
+      <c r="I40" s="40">
         <v>0.49490000000000001</v>
       </c>
-      <c r="J40" s="41">
+      <c r="J40" s="40">
         <v>8.9800000000000005E-2</v>
       </c>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41">
+      <c r="K40" s="40"/>
+      <c r="L40" s="40">
         <v>0.60870000000000002</v>
       </c>
-      <c r="M40" s="41">
+      <c r="M40" s="40">
         <v>0.10100000000000001</v>
       </c>
       <c r="O40" s="16" t="str">
@@ -6068,6 +6625,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="L14:M14"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="I26:J26"/>
@@ -6076,14 +6641,6 @@
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="L35:M35"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="L14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12594,4 +13151,213 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050DFD9F-3271-4AEA-A0CD-8C92AE406BFF}">
+  <dimension ref="C1:I22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1947</v>
+      </c>
+      <c r="D2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2">
+        <v>1947</v>
+      </c>
+      <c r="F2">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1959</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3">
+        <f>E2+5</f>
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1989</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E16" si="0">E3+5</f>
+        <v>1957</v>
+      </c>
+      <c r="F4">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1992</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2013</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2016</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2017</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1987</v>
+      </c>
+      <c r="F10">
+        <v>1989</v>
+      </c>
+      <c r="H10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1992</v>
+      </c>
+      <c r="F11">
+        <v>1992</v>
+      </c>
+      <c r="H11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>E13+5</f>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="F15">
+        <v>2013</v>
+      </c>
+      <c r="H15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="F16">
+        <v>2016</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>2017</v>
+      </c>
+      <c r="H17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="I22" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>